<commit_message>
Cost FR avec images (cor RMT)
</commit_message>
<xml_diff>
--- a/FR - Frame & Body/Cost/Cost_FR.xlsx
+++ b/FR - Frame & Body/Cost/Cost_FR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphaël\Desktop\ECL\2A\EPSA\Cost_Report_Vulcanix\Cost_FR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6512E51-4EF2-4B5D-8AFD-683BE2899ADC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A725B2CF-C511-4DF5-B949-AC150B84A54F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{3504F953-0384-4EFC-A842-97CB3EDD0BE8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" firstSheet="71" activeTab="76" xr2:uid="{3504F953-0384-4EFC-A842-97CB3EDD0BE8}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="5" r:id="rId1"/>
@@ -348,7 +348,7 @@
     <definedName name="FR_A0800_pa">'FR A0800'!$E$13</definedName>
     <definedName name="FR_A0800_q">'FR A0800'!$N$3</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2083,13 +2083,13 @@
     <numFmt numFmtId="183" formatCode="0.0000"/>
     <numFmt numFmtId="184" formatCode="0.00000"/>
     <numFmt numFmtId="185" formatCode="0.0000000"/>
-    <numFmt numFmtId="187" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* \-??_);_(@_)"/>
-    <numFmt numFmtId="188" formatCode="_-* #,##0.000\ _€_-;\-* #,##0.000\ _€_-;_-* &quot;-&quot;??????\ _€_-;_-@_-"/>
-    <numFmt numFmtId="189" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="190" formatCode="_-* #,##0.00000\ _€_-;\-* #,##0.00000\ _€_-;_-* &quot;-&quot;?????\ _€_-;_-@_-"/>
-    <numFmt numFmtId="192" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="193" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="194" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="186" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* \-??_);_(@_)"/>
+    <numFmt numFmtId="187" formatCode="_-* #,##0.000\ _€_-;\-* #,##0.000\ _€_-;_-* &quot;-&quot;??????\ _€_-;_-@_-"/>
+    <numFmt numFmtId="188" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="189" formatCode="_-* #,##0.00000\ _€_-;\-* #,##0.00000\ _€_-;_-* &quot;-&quot;?????\ _€_-;_-@_-"/>
+    <numFmt numFmtId="190" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="191" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="192" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="26" x14ac:knownFonts="1">
     <font>
@@ -3941,7 +3941,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="187" fontId="22" fillId="0" borderId="8" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="186" fontId="22" fillId="0" borderId="8" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="11" fontId="22" fillId="0" borderId="8" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="179" fontId="22" fillId="0" borderId="8" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="22" fillId="0" borderId="8" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -4049,7 +4049,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="188" fontId="22" fillId="0" borderId="47" xfId="16" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="187" fontId="22" fillId="0" borderId="47" xfId="16" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="39" xfId="16" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="47" xfId="16" applyBorder="1" applyAlignment="1"/>
@@ -4233,7 +4233,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="70" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="189" fontId="3" fillId="0" borderId="70" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="188" fontId="3" fillId="0" borderId="70" xfId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="71" xfId="16" applyFill="1" applyBorder="1"/>
@@ -4262,7 +4262,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="70" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="187" fontId="22" fillId="0" borderId="49" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="186" fontId="22" fillId="0" borderId="49" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="11" fontId="22" fillId="0" borderId="49" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="173" fontId="22" fillId="0" borderId="49" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="179" fontId="22" fillId="0" borderId="49" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -4285,7 +4285,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="73" xfId="16" applyFont="1" applyBorder="1"/>
     <xf numFmtId="182" fontId="22" fillId="0" borderId="24" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="180" fontId="22" fillId="0" borderId="24" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="190" fontId="22" fillId="0" borderId="24" xfId="16" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="189" fontId="22" fillId="0" borderId="24" xfId="16" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="22" fillId="0" borderId="24" xfId="16" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="22" fillId="0" borderId="8" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
@@ -4300,7 +4300,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="75" xfId="16" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="76" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="187" fontId="22" fillId="0" borderId="24" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="186" fontId="22" fillId="0" borderId="24" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="76" xfId="16" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="76" xfId="16" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4377,8 +4377,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="192" fontId="3" fillId="0" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="193" fontId="3" fillId="0" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="190" fontId="3" fillId="0" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="191" fontId="3" fillId="0" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="37" fontId="3" fillId="0" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -4389,7 +4389,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="194" fontId="3" fillId="0" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="192" fontId="3" fillId="0" borderId="24" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="19" fillId="2" borderId="56" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
@@ -4580,6 +4580,361 @@
 
 <file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>295276</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>63873</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>428626</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>137545</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BE4FEC7-B24B-4597-BCA7-AB56DCFEC267}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9420226" y="2349873"/>
+          <a:ext cx="1962150" cy="1597672"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>274321</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>111228</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7307579" cy="5585589"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0D77D0E-69EE-4A47-97B2-DE26AB2CF16A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="274321" y="301728"/>
+          <a:ext cx="7307579" cy="5585589"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>266701</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>533419</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>74685</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB987CA0-BD21-4531-BC59-32FCCF464BFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9429751" y="2390775"/>
+          <a:ext cx="2095518" cy="1493910"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>129541</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7774740" cy="5946374"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5F599CF-249D-42B2-9650-F16AF63882B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="129541" y="320040"/>
+          <a:ext cx="7774740" cy="5946374"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>82203</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>147000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB2C165B-86EC-4D98-9348-6186103A46F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9163050" y="2368203"/>
+          <a:ext cx="1819275" cy="1207797"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7225319" cy="5555846"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F095CDB-CFEF-4E15-A0F7-3EC2704A96C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="220980" y="358140"/>
+          <a:ext cx="7225319" cy="5555846"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>54202</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>108970</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90995884-07A7-45DC-B226-302E6D27A4E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7667625" y="2149702"/>
+          <a:ext cx="1247775" cy="1388268"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -4623,7 +4978,62 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>50534</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>145179</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7EB1CE4-48C8-4768-A755-D81A4D58208C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9153526" y="2146034"/>
+          <a:ext cx="1343024" cy="1428145"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -4657,366 +5067,6 @@
         <a:xfrm>
           <a:off x="228600" y="350520"/>
           <a:ext cx="7634575" cy="5847314"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="7781383" cy="5950187"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D281D34-F03E-49C3-B4BE-C406515CF98F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="175260" y="342900"/>
-          <a:ext cx="7781383" cy="5950187"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>350520</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="7332805" cy="5628238"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D30362D-B3DB-473A-8B9C-781E980D8440}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="350520" y="304800"/>
-          <a:ext cx="7332805" cy="5628238"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="7604554" cy="5843502"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{693A9792-BDB6-46BC-BE20-8AA4BA2FA106}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="228600" y="320040"/>
-          <a:ext cx="7604554" cy="5843502"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>335281</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="7930996" cy="6041627"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D419736-C310-432D-8877-1FBED8D44423}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="335281" y="335280"/>
-          <a:ext cx="7930996" cy="6041627"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>548641</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="7630220" cy="5830170"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{031F48E5-4EB5-40F7-A725-4A0113976050}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="548641" y="396240"/>
-          <a:ext cx="7630220" cy="5830170"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="7343583" cy="5635858"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{251918C2-2202-47A5-B03C-C9EC42290EA6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="304800" y="350520"/>
-          <a:ext cx="7343583" cy="5635858"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>251461</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="7445807" cy="5681578"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{152884B9-88BA-417D-B289-169CE8BB8D7F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="251461" y="342900"/>
-          <a:ext cx="7445807" cy="5681578"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="7529986" cy="5740634"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD5EF7C8-52A8-4B51-83D3-B93C81E4C564}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="228600" y="289560"/>
-          <a:ext cx="7529986" cy="5740634"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5085,65 +5135,25 @@
 
 <file path=xl/drawings/drawing20.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>320041</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>177241</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="7028925" cy="5374874"/>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>107319</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        <xdr:cNvPr id="3" name="Image 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{298BEC92-E378-4D31-999A-3AC94ED24BCC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="320041" y="259080"/>
-          <a:ext cx="7028925" cy="5374874"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing21.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1743075" cy="2883317"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5286D4E9-FDBA-4C09-983F-19FEB5E9F035}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C802BB3-1428-4D80-AF9D-D8BF6AEA58C6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5165,8 +5175,53 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3667125" y="47625"/>
-          <a:ext cx="1743075" cy="2883317"/>
+          <a:off x="7711516" y="2543174"/>
+          <a:ext cx="2997128" cy="1857376"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing21.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7781383" cy="5950187"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D281D34-F03E-49C3-B4BE-C406515CF98F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="175260" y="342900"/>
+          <a:ext cx="7781383" cy="5950187"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5180,20 +5235,25 @@
 
 <file path=xl/drawings/drawing22.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>121584</xdr:rowOff>
+      <xdr:colOff>107769</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2562612" cy="2007534"/>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>448322</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>93748</xdr:rowOff>
+    </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
+        <xdr:cNvPr id="3" name="Image 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27695709-D126-4319-87EA-C5062D945E73}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6571B988-D714-44D7-B33B-08755A2A209C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5215,8 +5275,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9123269" y="2407584"/>
-          <a:ext cx="2562612" cy="2007534"/>
+          <a:off x="8737419" y="2171700"/>
+          <a:ext cx="1578803" cy="1351048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5224,7 +5284,7 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:oneCellAnchor>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5233,17 +5293,18 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4324350" cy="3064274"/>
+    <xdr:ext cx="7332805" cy="5628238"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Image 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20AA8472-CEA6-4BDE-8C31-D26EEE0080F6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D30362D-B3DB-473A-8B9C-781E980D8440}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5252,21 +5313,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="381001"/>
-          <a:ext cx="4324350" cy="3064274"/>
+          <a:off x="350520" y="304800"/>
+          <a:ext cx="7332805" cy="5628238"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5280,70 +5335,25 @@
 
 <file path=xl/drawings/drawing24.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>155421</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>152984</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1352074" cy="1093304"/>
+      <xdr:colOff>446718</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>124266</xdr:rowOff>
+    </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
+        <xdr:cNvPr id="3" name="Image 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCA18504-C626-43B0-AF36-C9237A23E7ED}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10980303" y="2438984"/>
-          <a:ext cx="1352074" cy="1093304"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing25.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>351384</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>181694</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="3367876" cy="2812489"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21A633A3-4B71-475B-8B46-74E3379EB4D3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11BDB581-D189-4C09-88F2-79B73F0FC0C8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5365,8 +5375,53 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7114134" y="181694"/>
-          <a:ext cx="3367876" cy="2812489"/>
+          <a:off x="9105900" y="2152649"/>
+          <a:ext cx="1427793" cy="1400617"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing25.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7604554" cy="5843502"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{693A9792-BDB6-46BC-BE20-8AA4BA2FA106}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="228600" y="320040"/>
+          <a:ext cx="7604554" cy="5843502"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5380,20 +5435,25 @@
 
 <file path=xl/drawings/drawing26.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>149680</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>149679</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1038224</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>79183</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1551214" cy="1892765"/>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2238375</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>151444</xdr:rowOff>
+    </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
+        <xdr:cNvPr id="3" name="Image 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2ADE4192-0EEB-471D-B35B-820309BD9FDA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B781C0BF-F199-4D3E-A793-B8AF80756101}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5402,10 +5462,10 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -5415,8 +5475,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10463894" y="2435679"/>
-          <a:ext cx="1551214" cy="1892765"/>
+          <a:off x="6457949" y="79183"/>
+          <a:ext cx="1200151" cy="1596261"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5424,7 +5484,7 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:oneCellAnchor>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5432,18 +5492,19 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>335281</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2667223" cy="895351"/>
+    <xdr:ext cx="7930996" cy="6041627"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Image 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47FA5777-73A5-494B-A714-AAB9CC418C7F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D419736-C310-432D-8877-1FBED8D44423}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5452,21 +5513,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5857875" y="2943224"/>
-          <a:ext cx="2667223" cy="895351"/>
+          <a:off x="335281" y="335280"/>
+          <a:ext cx="7930996" cy="6041627"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5480,20 +5535,25 @@
 
 <file path=xl/drawings/drawing28.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>390526</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1434193" cy="711171"/>
+      <xdr:colOff>452033</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
+        <xdr:cNvPr id="3" name="Image 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{427BB75C-B48A-4A05-8834-257345A865EB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0B4FD03-603C-4001-9A82-44B65C773948}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5502,10 +5562,10 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -5515,8 +5575,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7096126" y="2533650"/>
-          <a:ext cx="1434193" cy="711171"/>
+          <a:off x="9039226" y="2143125"/>
+          <a:ext cx="1480732" cy="1390649"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5524,7 +5584,7 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:oneCellAnchor>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5532,18 +5592,19 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>548641</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1506074" cy="1257299"/>
+    <xdr:ext cx="7630220" cy="5830170"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Image 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29D1BEA0-C44F-495D-A49E-BF62E9A7D8D6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{031F48E5-4EB5-40F7-A725-4A0113976050}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5552,21 +5613,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7058025" y="2476501"/>
-          <a:ext cx="1506074" cy="1257299"/>
+          <a:off x="548641" y="396240"/>
+          <a:ext cx="7630220" cy="5830170"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5635,6 +5690,966 @@
 
 <file path=xl/drawings/drawing30.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>212074</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>45102</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>64580</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD39880B-6E75-410B-AED8-ABA5B92873B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="5425536" y="22765"/>
+          <a:ext cx="1162478" cy="1969151"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing31.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7343583" cy="5635858"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{251918C2-2202-47A5-B03C-C9EC42290EA6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="304800" y="350520"/>
+          <a:ext cx="7343583" cy="5635858"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing32.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>166202</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89C13CBA-FB21-496D-8EA0-EDB8844B466D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9423400" y="3492500"/>
+          <a:ext cx="3087202" cy="1879600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing33.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>58919</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>50801</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>579471</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>139701</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3016FE1-10A2-4B9F-97B8-7A69FF8DC2E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7615419" y="2146301"/>
+          <a:ext cx="1739752" cy="1231900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing34.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>251461</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7445807" cy="5681578"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{152884B9-88BA-417D-B289-169CE8BB8D7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="251461" y="342900"/>
+          <a:ext cx="7445807" cy="5681578"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing35.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>179293</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>50545</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>388117</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{293A81B0-F89B-4127-B801-DC5101F58571}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9143999" y="2336545"/>
+          <a:ext cx="2263589" cy="1290072"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing36.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7529986" cy="5740634"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD5EF7C8-52A8-4B51-83D3-B93C81E4C564}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="228600" y="289560"/>
+          <a:ext cx="7529986" cy="5740634"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing37.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>98272</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>108850</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FEA6A29-C8D9-48F9-AF01-A30B0F68D471}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6115050" y="123825"/>
+          <a:ext cx="1460347" cy="1509025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing38.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>320041</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7028925" cy="5374874"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{298BEC92-E378-4D31-999A-3AC94ED24BCC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="320041" y="259080"/>
+          <a:ext cx="7028925" cy="5374874"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing39.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1743075" cy="2883317"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5286D4E9-FDBA-4C09-983F-19FEB5E9F035}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3667125" y="47625"/>
+          <a:ext cx="1743075" cy="2883317"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>500063</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>169073</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{522F3C6B-0D65-4A37-97A5-BB6E898D0BF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8620126" y="1309687"/>
+          <a:ext cx="4622010" cy="3286125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing40.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>121584</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2562612" cy="2007534"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27695709-D126-4319-87EA-C5062D945E73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9123269" y="2407584"/>
+          <a:ext cx="2562612" cy="2007534"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing41.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4324350" cy="3064274"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20AA8472-CEA6-4BDE-8C31-D26EEE0080F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="381001"/>
+          <a:ext cx="4324350" cy="3064274"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing42.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>155421</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152984</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1352074" cy="1093304"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCA18504-C626-43B0-AF36-C9237A23E7ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10980303" y="2438984"/>
+          <a:ext cx="1352074" cy="1093304"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing43.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>351384</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>181694</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3367876" cy="2812489"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21A633A3-4B71-475B-8B46-74E3379EB4D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7114134" y="181694"/>
+          <a:ext cx="3367876" cy="2812489"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing44.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>149680</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>149679</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1551214" cy="1892765"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2ADE4192-0EEB-471D-B35B-820309BD9FDA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10463894" y="2435679"/>
+          <a:ext cx="1551214" cy="1892765"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing45.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2667223" cy="895351"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47FA5777-73A5-494B-A714-AAB9CC418C7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5857875" y="2943224"/>
+          <a:ext cx="2667223" cy="895351"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing46.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>390526</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1434193" cy="711171"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{427BB75C-B48A-4A05-8834-257345A865EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7096126" y="2533650"/>
+          <a:ext cx="1434193" cy="711171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing47.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1506074" cy="1257299"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29D1BEA0-C44F-495D-A49E-BF62E9A7D8D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7058025" y="2476501"/>
+          <a:ext cx="1506074" cy="1257299"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing48.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -5683,7 +6698,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing49.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -5733,7 +6748,52 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7478744" cy="5693015"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38C5D56F-0A4E-4CA6-A98C-79F025B57DE6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="441960" y="304800"/>
+          <a:ext cx="7478744" cy="5693015"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing50.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -5783,7 +6843,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing51.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -5833,7 +6893,117 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing52.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>266701</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>110367</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>444501</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>63501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{456324C1-4080-4BC1-84A9-749D01741BA1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8826501" y="1253367"/>
+          <a:ext cx="3314700" cy="2251834"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing53.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>63501</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>196237</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>46120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D074519-D79A-46DD-87F3-9BBEE82E6366}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8051801" y="2552700"/>
+          <a:ext cx="3333136" cy="2636920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing54.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -5878,7 +7048,62 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing55.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>212914</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>73619</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>277936</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B17649F3-5610-4476-BB2F-F044FA7CA130}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7631208" y="2359619"/>
+          <a:ext cx="2485493" cy="1775352"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing56.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -5923,7 +7148,62 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing57.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>156883</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>26332</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>493059</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>155362</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33C1E904-184E-4C81-B357-7FDE6871962D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8303559" y="2312332"/>
+          <a:ext cx="2151529" cy="1843530"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing58.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -5968,7 +7248,117 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing59.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>163285</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>39136</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>544285</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>168018</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7D9914B-AFC0-4396-92F8-901453648D3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9375321" y="2515636"/>
+          <a:ext cx="2898321" cy="1652882"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>369794</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>459441</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>115858</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADAE8C26-6315-4150-829C-41C45FD0ABDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8942294" y="2173941"/>
+          <a:ext cx="1299882" cy="2704417"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing60.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -6013,7 +7403,62 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing61.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>299358</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>149679</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>147410</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF110C31-3609-494B-B25F-9F0F6A0323AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9497787" y="2503714"/>
+          <a:ext cx="2367642" cy="1644196"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing62.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -6058,7 +7503,62 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing63.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1133475</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>89040</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6A04C48-3D8A-431A-8D94-BA67D7E1BAEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6486525" y="66675"/>
+          <a:ext cx="1400175" cy="1546365"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing64.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -6103,23 +7603,27 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing65.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1095375</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="7478744" cy="5693015"/>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>93768</xdr:rowOff>
+    </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        <xdr:cNvPr id="3" name="Image 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38C5D56F-0A4E-4CA6-A98C-79F025B57DE6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEC78E91-6B98-4195-8859-321DC6298953}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6128,15 +7632,21 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="441960" y="304800"/>
-          <a:ext cx="7478744" cy="5693015"/>
+          <a:off x="6143625" y="123825"/>
+          <a:ext cx="1914525" cy="1493943"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6144,11 +7654,11 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:oneCellAnchor>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing66.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -6193,7 +7703,62 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing67.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1038226</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>29173</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>409576</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>146904</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E48AC837-392A-403B-A0F4-104C51E08FFD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6324601" y="29173"/>
+          <a:ext cx="2381250" cy="1641731"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing68.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -6238,7 +7803,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -6283,7 +7848,62 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>371476</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>415884</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>107639</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B64C0AD5-6C60-4591-8A6D-A7506BB47F3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8191501" y="2143125"/>
+          <a:ext cx="654008" cy="2155514"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -6317,141 +7937,6 @@
         <a:xfrm>
           <a:off x="205740" y="403860"/>
           <a:ext cx="8141479" cy="6211170"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>274321</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>111228</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="7307579" cy="5585589"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0D77D0E-69EE-4A47-97B2-DE26AB2CF16A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="274321" y="301728"/>
-          <a:ext cx="7307579" cy="5585589"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>129541</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="7774740" cy="5946374"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5F599CF-249D-42B2-9650-F16AF63882B9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="129541" y="320040"/>
-          <a:ext cx="7774740" cy="5946374"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="7225319" cy="5555846"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F095CDB-CFEF-4E15-A0F7-3EC2704A96C5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="220980" y="358140"/>
-          <a:ext cx="7225319" cy="5555846"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7744,12 +9229,12 @@
   </sheetPr>
   <dimension ref="A1:O205"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="6" topLeftCell="D22" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="6" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
       <selection activeCell="H10" sqref="H10"/>
       <selection pane="topRight" activeCell="H10" sqref="H10"/>
       <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
-      <selection pane="bottomRight" activeCell="F63" sqref="F63"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12770,8 +14255,8 @@
   </sheetPr>
   <dimension ref="A1:O112"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="J107" sqref="J107"/>
+    <sheetView zoomScale="40" zoomScaleNormal="40" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16257,6 +17742,7 @@
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="111" max="16383" man="1"/>
   </rowBreaks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -16269,7 +17755,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16897,8 +18383,8 @@
   </sheetPr>
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17534,6 +19020,7 @@
     <hyperlink ref="G2" location="FR_A0300_BOM" display="Back to BOM" xr:uid="{3D63613C-F120-4331-94D8-F5088F0E0BDA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -17579,7 +19066,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18148,6 +19635,7 @@
     <hyperlink ref="G2" location="FR_A0300_BOM" display="Back to BOM" xr:uid="{088F383E-3347-4CD8-A27C-73EB7905C1DE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -18193,7 +19681,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18768,6 +20256,7 @@
     <hyperlink ref="G2" location="FR_A0300_BOM" display="Back to BOM" xr:uid="{D22301CA-87FB-4606-9ADD-78A77B52DFD4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -18811,7 +20300,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19386,6 +20875,7 @@
     <hyperlink ref="G2" location="FR_A0300_BOM" display="Back to BOM" xr:uid="{091E754E-C2A5-4C9B-8F15-FB37BD583945}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -20508,7 +21998,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21017,6 +22507,7 @@
     <hyperlink ref="G2" location="FR_A0300_BOM" display="Back to BOM" xr:uid="{59738A87-E595-4435-904B-6FA95449091F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -21061,7 +22552,7 @@
   <dimension ref="A1:XFD19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33872,6 +35363,7 @@
     <hyperlink ref="G2" location="FR_A0300_BOM" display="Back to BOM" xr:uid="{AE0BC1BB-AF45-4236-BF19-2B09FEA8F186}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -34427,6 +35919,7 @@
     <hyperlink ref="G2" location="FR_A0300_BOM" display="Back to BOM" xr:uid="{3B6E7F87-68CC-4FC6-A34B-91D4ED223CDD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -34469,7 +35962,7 @@
   </sheetPr>
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
@@ -35123,6 +36616,7 @@
     <hyperlink ref="G2" location="FR_A0300_BOM" display="Back to BOM" xr:uid="{755FB99F-DA0C-41F6-8E6F-2AD3F3CE69EF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -35169,7 +36663,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35678,6 +37172,7 @@
     <hyperlink ref="G2" location="FR_A0300_BOM" display="Back to BOM" xr:uid="{A93118B2-5413-426D-B9E9-E85AF24F2CE6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -36870,6 +38365,7 @@
     <hyperlink ref="G2" location="FR_A0300_BOM" display="Back to BOM" xr:uid="{96BE8E58-F450-43A7-81C2-C70DA589553F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -37418,6 +38914,7 @@
     <hyperlink ref="G2" location="FR_A0300_BOM" display="Back to BOM" xr:uid="{FBA7EB99-84EF-4622-95B9-B27A44CDD8AD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -37463,7 +38960,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37968,6 +39465,7 @@
     <hyperlink ref="G2" location="FR_A0300_BOM" display="Back to BOM" xr:uid="{409340EA-D033-4A31-A962-09F94EC619B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -38013,7 +39511,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38514,6 +40012,7 @@
     <hyperlink ref="G2" location="FR_A0300_BOM" display="Back to BOM" xr:uid="{C7715EBA-F710-43FC-9E36-D005FF921B7E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -38525,7 +40024,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38558,8 +40057,8 @@
   </sheetPr>
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39691,6 +41190,7 @@
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="39" max="16383" man="1"/>
   </rowBreaks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -40020,7 +41520,7 @@
       </c>
       <c r="O11" s="194"/>
     </row>
-    <row r="12" spans="1:15" s="164" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" s="164" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="205">
         <v>20</v>
       </c>
@@ -40502,7 +42002,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41013,6 +42513,7 @@
     <brk id="18" max="16383" man="1"/>
     <brk id="52" max="16383" man="1"/>
   </rowBreaks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -41062,7 +42563,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41538,7 +43039,7 @@
       <c r="N17" s="135"/>
       <c r="O17" s="134"/>
     </row>
-    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="133"/>
       <c r="B18" s="132"/>
       <c r="C18" s="132"/>
@@ -41562,6 +43063,7 @@
     <hyperlink ref="G2" location="FR_A0400_BOM" display="Back to BOM" xr:uid="{1F7D7AE0-EFDE-4B73-9D6D-899FDA809C11}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -41609,7 +43111,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42113,6 +43615,7 @@
     <hyperlink ref="G2" location="FR_A0400_BOM" display="Back to BOM" xr:uid="{7B440420-9304-4014-91D6-0B5D4D952ED9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -49285,7 +50788,7 @@
         <v>1</v>
       </c>
       <c r="I57" s="140">
-        <f t="shared" ref="I57:I88" si="3">IF(H57="",D57*F57,D57*F57*H57)</f>
+        <f t="shared" ref="I57:I78" si="3">IF(H57="",D57*F57,D57*F57*H57)</f>
         <v>6.25E-2</v>
       </c>
       <c r="J57" s="139"/>
@@ -50244,7 +51747,7 @@
       <c r="N85" s="190"/>
       <c r="O85" s="134"/>
     </row>
-    <row r="86" spans="1:15" s="447" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" s="447" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="455">
         <v>50</v>
       </c>
@@ -54947,7 +56450,7 @@
   <dimension ref="A1:O58"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56645,6 +58148,7 @@
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="57" max="16383" man="1"/>
   </rowBreaks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -56657,7 +58161,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57436,6 +58940,7 @@
     <brk id="24" max="16383" man="1"/>
     <brk id="58" max="16383" man="1"/>
   </rowBreaks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -58123,6 +59628,7 @@
     <hyperlink ref="G2" location="FR_A0700_BOM" display="Back to BOM" xr:uid="{83CC60D7-0523-4E68-837F-B1680CD40A33}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -58807,6 +60313,7 @@
     <hyperlink ref="G2" location="FR_A0700_BOM" display="Back to BOM" xr:uid="{3A1C8B3A-35B1-445F-BA49-42AF70C3B133}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -58852,7 +60359,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59506,6 +61013,7 @@
     <hyperlink ref="G2" location="FR_A0700_BOM" display="Back to BOM" xr:uid="{083A7BF5-BFF9-4264-BBAA-A18CD741C049}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -59552,7 +61060,7 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -60241,6 +61749,7 @@
     <hyperlink ref="G2" location="FR_A0700_BOM" display="Back to BOM" xr:uid="{61AD78D5-BA65-4466-8F64-C13E0AA41827}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -60795,6 +62304,7 @@
     <hyperlink ref="G2" location="FR_A0700_BOM" display="Back to BOM" xr:uid="{118DCDC4-E2CC-4918-B3B7-6D59F91D38C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -60840,7 +62350,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -61349,6 +62859,7 @@
     <hyperlink ref="G2" location="FR_A0700_BOM" display="Back to BOM" xr:uid="{AD7B8D4C-9747-420C-8583-0EF5AEC7911A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -61393,8 +62904,8 @@
   </sheetPr>
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -61902,6 +63413,7 @@
     <hyperlink ref="G2" location="FR_A0700_BOM" display="Back to BOM" xr:uid="{E897A953-3CEE-4746-9474-F19C3587E3E5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -62510,7 +64022,7 @@
         <v>1</v>
       </c>
       <c r="I21" s="563">
-        <f>D21*F21*H21</f>
+        <f t="shared" ref="I21:I27" si="0">D21*F21*H21</f>
         <v>0.26</v>
       </c>
       <c r="J21" s="559"/>
@@ -62544,7 +64056,7 @@
         <v>1.5</v>
       </c>
       <c r="I22" s="563">
-        <f>D22*F22*H22</f>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="J22" s="559"/>
@@ -62576,7 +64088,7 @@
         <v>1</v>
       </c>
       <c r="I23" s="560">
-        <f>D23*F23*H23</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="J23" s="4"/>
@@ -62608,7 +64120,7 @@
         <v>1</v>
       </c>
       <c r="I24" s="560">
-        <f>D24*F24*H24</f>
+        <f t="shared" si="0"/>
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="J24" s="4"/>
@@ -62640,7 +64152,7 @@
         <v>1</v>
       </c>
       <c r="I25" s="560">
-        <f>D25*F25*H25</f>
+        <f t="shared" si="0"/>
         <v>0.26</v>
       </c>
       <c r="J25" s="4"/>
@@ -62672,7 +64184,7 @@
         <v>1</v>
       </c>
       <c r="I26" s="560">
-        <f>D26*F26*H26</f>
+        <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
       <c r="J26" s="4"/>
@@ -62704,7 +64216,7 @@
         <v>1</v>
       </c>
       <c r="I27" s="560">
-        <f>D27*F27*H27</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J27" s="4"/>

</xml_diff>